<commit_message>
Fix reference numbering for Articles
</commit_message>
<xml_diff>
--- a/MissingReferences.xlsx
+++ b/MissingReferences.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="1088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="1100">
   <si>
     <t xml:space="preserve">Articles</t>
   </si>
@@ -2378,10 +2378,13 @@
     <t xml:space="preserve">[30] Lin VC, Ng EH, Aw SE, Tan MG, Ng EH, Chan VS, Ho GH. Progestins inhibit the growth of MDA-MB-231 cells transfected with progesterone receptor complementary DNA. Clin Cancer Res. 1999 Feb;5(2):395-403. PMID: 10037189. </t>
   </si>
   <si>
-    <t xml:space="preserve">[38] Macaione S, Ientile R, Lentini M, Di Giorgio RM. Effects of estrogens and progesterone on GABA system in ovariectomized rat retina. Ital J Biochem. 1981 Jul-Aug;30(4):279-89. PMID: 7298312. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[40] Mauvais-Jarvis P, Gompel A, Malet C, Kuttenn F. Antiestrogènes et prolifération cellulaire mammaire normale humaine [Antiestrogens and normal human breast cell proliferation]. Ann Endocrinol (Paris). 1989;50(3):181-8. French. PMID: 2683973. </t>
+    <t xml:space="preserve">[33] Lin VC, Ng EH, Aw SE, Tan MG, Ng EH, Chan VS, Ho GH. Progestins inhibit the growth of MDA-MB-231 cells transfected with progesterone receptor complementary DNA. Clin Cancer Res. 1999 Feb;5(2):395-403. PMID: 10037189. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[39] Macaione S, Ientile R, Lentini M, Di Giorgio RM. Effects of estrogens and progesterone on GABA system in ovariectomized rat retina. Ital J Biochem. 1981 Jul-Aug;30(4):279-89. PMID: 7298312. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[41] Mauvais-Jarvis P, Gompel A, Malet C, Kuttenn F. Antiestrogènes et prolifération cellulaire mammaire normale humaine [Antiestrogens and normal human breast cell proliferation]. Ann Endocrinol (Paris). 1989;50(3):181-8. French. PMID: 2683973. </t>
   </si>
   <si>
     <r>
@@ -2702,6 +2705,36 @@
     <t xml:space="preserve">[14] Dyro FM. Quadriparesis as an unusual manifestation of hypercalcemia. J Maine Med Assoc. 1977 Oct;68(10):370-1. PMID: 908889. </t>
   </si>
   <si>
+    <t xml:space="preserve">[21] Gannagé-Yared MH, Tohmé A, Halaby G. L'hypovitaminose D, problème mondial majeur de santé publique [Hypovitaminosis D: a major worldwide public health problem]. Presse Med. 2001 Apr 7;30(13):653-8. French. PMID: 11346909. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[27] Grecu EO, Weinshelbaum A, Simmons R. Effective therapy of glucocorticoid-induced osteoporosis with medroxyprogesterone acetate. Calcif Tissue Int. 1990 May;46(5):294-9. doi: 10.1007/BF02563818. PMID: 2140069. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[29] Haas PJ. Antiallergische Wirkung von Kalzium per os. Eine klinisch-experimentelle Studie [Antiallergic effect of oral calcium. A clinico-experimental study]. Fortschr Med. 1985 Mar 28;103(12):328-30. German. PMID: 3872822. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[30] Hilgard P, Hohage R, Schmitt W, Minne H, Ziegler R. The possible role of platelets as trigger in intravascular coagulation associated with acute hyperparathyroidism. Acta Univ Carol Med Monogr. 1972;53:427-32. PMID: 4670750. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[34] Massry SG. Pathogenesis of the anemia of uremia: role of secondary hyperparathyroidism. Kidney Int Suppl. 1983 Dec;16:S204-7. PMID: 6376915. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[49] Ouchi Y, Orimo H. [Calcium and magnesium metabolism in the aged]. Nihon Ronen Igakkai Zasshi. 1989 May;26(3):216-22. Japanese. PMID: 2795971. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[59] Rude RK, Kirchen ME, Gruber HE, Meyer MH, Luck JS, Crawford DL. Magnesium deficiency-induced osteoporosis in the rat: uncoupling of bone formation and bone resorption. Magnes Res. 1999 Dec;12(4):257-67. PMID: 10612083. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[60] Schmid C. Hyperkalzämie [Hypercalcemia]. Schweiz Med Wochenschr. 1994 Jun 25;124(25):1122-8. German. PMID: 8029686. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[69] Utz G, Hauck AM. Orale anwendung von Kalzium plus Vitamin D2 bei allergischem Asthma bronchiale [Oral application of calcium and vitamin D2 in allergic bronchial asthma (author's transl)]. MMW Munch Med Wochenschr. 1976 Oct 22;118(43):1395-8. German. PMID: 825744. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[76] Zofková I, Kanceva RL. Nové látky s pozitivním úcinkem na kost [New drugs with positive effects on bones]. Cas Lek Cesk. 1997 Jul 30;136(15):459-63. Czech. PMID: 9340191. </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -2831,10 +2864,10 @@
     <t xml:space="preserve">[61] Pozharisskaia TD, Vasil'eva TP, Sokolova EN, Alekseeva II. K mekhanizmu rasstroĭstv krovoobrashcheniia u zhivotnykh, obluchennykh v bol'shih dozakh [Mechanism of circulatory disorders in animals irradiated at high doses]. Radiobiologiia. 1985 Nov-Dec;25(6):763-7. Russian. PMID: 4080994. </t>
   </si>
   <si>
-    <t xml:space="preserve">[68] Smídová L, Base J, Mourek J, Cechová I. Proportion of individual fatty acids in the non-esterified (free) fatty acid (FFA) fraction in the serum of laboratory rats of different ages. Physiol Bohemoslov. 1990;39(2):125-34. PMID: 2144352. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[70] Staub F, Winkler A, Peters J, Kempski O, Baethmann A. Mechanisms of glial swelling by arachidonic acid. Acta Neurochir Suppl (Wien). 1994;60:20-3. doi: 10.1007/978-3-7091-9334-1_5. PMID: 7976545. </t>
+    <t xml:space="preserve">[69] Smídová L, Base J, Mourek J, Cechová I. Proportion of individual fatty acids in the non-esterified (free) fatty acid (FFA) fraction in the serum of laboratory rats of different ages. Physiol Bohemoslov. 1990;39(2):125-34. PMID: 2144352. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[71] Staub F, Winkler A, Peters J, Kempski O, Baethmann A. Mechanisms of glial swelling by arachidonic acid. Acta Neurochir Suppl (Wien). 1994;60:20-3. doi: 10.1007/978-3-7091-9334-1_5. PMID: 7976545. </t>
   </si>
   <si>
     <r>
@@ -3537,6 +3570,9 @@
   </si>
   <si>
     <t xml:space="preserve">[20] D. Green-Kelly, B.V. Derjaguin, Research in Surface Forces vol. 2, p. 117, Consultants Bureau, NY (1966).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[24] McIntyre GI. Increased cell hydration promotes both tumor growth and metastasis: a biochemical mechanism consistent with genetic signatures. Med Hypotheses. 2007;69(5):1127-30. doi: 10.1016/j.mehy.2007.01.080. Epub 2007 Mar 30. PMID: 17399912. </t>
   </si>
   <si>
     <r>
@@ -4042,19 +4078,19 @@
     <t xml:space="preserve">[22] Merk FB, Warhol MJ, Kwan PW, Leav I, Alroy J, Ofner P, Pinkus GS. Multiple phenotypes of prostatic glandular cells in castrated dogs after individual or combined treatment with androgen and estrogen. Morphometric, ultrastructural, and cytochemical distinctions. Lab Invest. 1986 Apr;54(4):442-56. PMID: 2421104. </t>
   </si>
   <si>
-    <t xml:space="preserve">[25] Rolland PH, Martin PM, Jacquemier J, Rolland AM, Toga M. Prostaglandin in human breast cancer: Evidence suggesting that an elevated prostaglandin production is a marker of high metastatic potential for neoplastic cells. J Natl Cancer Inst. 1980 May;64(5):1061-70. PMID: 6767871. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[27] Schuman LM, Mandel J, Blackard C, Bauer H, Scarlett J, McHugh R. Epidemiologic study of prostatic cancer: preliminary report. Cancer Treat Rep. 1977 Mar-Apr;61(2):181-6. PMID: 194689. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[28] Siiteri, P.K. and P. C. MacDonald, "Role of extraglandular estrogen in human endocrinology," In Handbook of Physiology, section 7, Endocrinology Vol II (Eds. S. R. Geiger, et al.,) pp. 615-629, Williams &amp; Wilkins, Baltimore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[31] TULLNER WW. HORMONAL FACTORS IN THE ADRENAL-DEPENDENT GROWTH OF THE RAT VENTRAL PROSTATE. Natl Cancer Inst Monogr. 1963 Oct;12:211-23. PMID: 14072993. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[35] Vermeulen, A. "Hormonal factors related to abnormal growth of the prostate." Prostate Cancer. 48 (1979): 81-92.  UICC, Geneva</t>
+    <t xml:space="preserve">[24] Rolland PH, Martin PM, Jacquemier J, Rolland AM, Toga M. Prostaglandin in human breast cancer: Evidence suggesting that an elevated prostaglandin production is a marker of high metastatic potential for neoplastic cells. J Natl Cancer Inst. 1980 May;64(5):1061-70. PMID: 6767871. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[26] Schuman LM, Mandel J, Blackard C, Bauer H, Scarlett J, McHugh R. Epidemiologic study of prostatic cancer: preliminary report. Cancer Treat Rep. 1977 Mar-Apr;61(2):181-6. PMID: 194689. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[27] Siiteri, P.K. and P. C. MacDonald, "Role of extraglandular estrogen in human endocrinology," In Handbook of Physiology, section 7, Endocrinology Vol II (Eds. S. R. Geiger, et al.,) pp. 615-629, Williams &amp; Wilkins, Baltimore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[30] TULLNER WW. HORMONAL FACTORS IN THE ADRENAL-DEPENDENT GROWTH OF THE RAT VENTRAL PROSTATE. Natl Cancer Inst Monogr. 1963 Oct;12:211-23. PMID: 14072993. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[34] Vermeulen, A. "Hormonal factors related to abnormal growth of the prostate." Prostate Cancer. 48 (1979): 81-92.  UICC, Geneva</t>
   </si>
   <si>
     <r>
@@ -4270,16 +4306,16 @@
     <t xml:space="preserve">[14] THE DAILY CITIZEN, April 5, 1994. Robert Greene, "Soggy Chickens," AP, April 2, 1994; "Interview with Elaine Dodge,"</t>
   </si>
   <si>
-    <t xml:space="preserve">[17] Ideta T. [Studies on relationship between progressive muscular dystrophy and estrogen]. Kumamoto Igakkai Zasshi. 1969 Aug 25;43(8):661-80. Japanese. PMID: 5395315. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[21] Jonkman JH, Westenberg HG, Rijntjes NV, van der Kleijn E, Lindeboom SF. Whole body distribution of the quaternary ammonium compound thiazinamium (N-methylpromethazine) and promethazine in monkey and mice. Arzneimittelforschung. 1983;33(2):223-8. PMID: 6133524. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[23] Kovach JS, Svingen PA. Enhancement of the antiproliferative activity of human interferon by polyamine depletion. Cancer Treat Rep. 1985 Jan;69(1):97-103. PMID: 3917854. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[25] Kuchár S, Mozes S, Boda K, Koppel J. The effect of androgen and estrogen on food intake and body weight in rats--age dependency. Endokrinologie. 1982 Nov;80(3):294-8. PMID: 7166161. </t>
+    <t xml:space="preserve">[16] Ideta T. [Studies on relationship between progressive muscular dystrophy and estrogen]. Kumamoto Igakkai Zasshi. 1969 Aug 25;43(8):661-80. Japanese. PMID: 5395315. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[20] Jonkman JH, Westenberg HG, Rijntjes NV, van der Kleijn E, Lindeboom SF. Whole body distribution of the quaternary ammonium compound thiazinamium (N-methylpromethazine) and promethazine in monkey and mice. Arzneimittelforschung. 1983;33(2):223-8. PMID: 6133524. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[22] Kovach JS, Svingen PA. Enhancement of the antiproliferative activity of human interferon by polyamine depletion. Cancer Treat Rep. 1985 Jan;69(1):97-103. PMID: 3917854. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[24] Kuchár S, Mozes S, Boda K, Koppel J. The effect of androgen and estrogen on food intake and body weight in rats--age dependency. Endokrinologie. 1982 Nov;80(3):294-8. PMID: 7166161. </t>
   </si>
   <si>
     <t xml:space="preserve">[27] Lewis JS, Vijayanathan V, Thomas TJ, Pestell RG, Albanese C, Gallo MA, Thomas T. Activation of cyclin D1 by estradiol and spermine in MCF-7 breast cancer cells: a mechanism involving the p38 MAP kinase and phosphorylation of ATF-2. Oncol Res. 2005;15(3):113-28. doi: 10.3727/096504005776367924. PMID: 16050133. </t>
@@ -7129,8 +7165,8 @@
   </sheetPr>
   <dimension ref="A1:BH98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O52" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P53" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7180,7 +7216,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="63" style="2" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7328,7 +7364,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>48</v>
       </c>
@@ -7390,7 +7426,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
@@ -7482,7 +7518,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>98</v>
       </c>
@@ -7523,7 +7559,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>111</v>
       </c>
@@ -7531,7 +7567,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="73.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>113</v>
       </c>
@@ -7542,7 +7578,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="61.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>116</v>
       </c>
@@ -7556,7 +7592,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="73.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>120</v>
       </c>
@@ -7585,7 +7621,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>129</v>
       </c>
@@ -7608,7 +7644,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>136</v>
       </c>
@@ -7664,7 +7700,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>154</v>
       </c>
@@ -7714,7 +7750,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>170</v>
       </c>
@@ -7737,7 +7773,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>177</v>
       </c>
@@ -7790,7 +7826,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="265.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="291.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>194</v>
       </c>
@@ -7828,7 +7864,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>206</v>
       </c>
@@ -7875,7 +7911,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>221</v>
       </c>
@@ -7913,7 +7949,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>233</v>
       </c>
@@ -7937,7 +7973,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>240</v>
       </c>
@@ -7951,7 +7987,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>244</v>
       </c>
@@ -7980,7 +8016,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>253</v>
       </c>
@@ -8003,7 +8039,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>260</v>
       </c>
@@ -8038,7 +8074,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>271</v>
       </c>
@@ -8055,7 +8091,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>276</v>
       </c>
@@ -8093,7 +8129,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>288</v>
       </c>
@@ -8132,7 +8168,7 @@
       </c>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>300</v>
       </c>
@@ -8155,7 +8191,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>307</v>
       </c>
@@ -8199,7 +8235,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>321</v>
       </c>
@@ -8255,7 +8291,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="162" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>339</v>
       </c>
@@ -8395,7 +8431,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>385</v>
       </c>
@@ -8430,7 +8466,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>396</v>
       </c>
@@ -8441,7 +8477,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>399</v>
       </c>
@@ -8464,7 +8500,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="61.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>406</v>
       </c>
@@ -8490,7 +8526,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>414</v>
       </c>
@@ -8507,7 +8543,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>419</v>
       </c>
@@ -8530,7 +8566,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>426</v>
       </c>
@@ -8562,7 +8598,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>436</v>
       </c>
@@ -8591,7 +8627,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>445</v>
       </c>
@@ -8626,7 +8662,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>456</v>
       </c>
@@ -8652,7 +8688,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="49.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>464</v>
       </c>
@@ -8666,7 +8702,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>468</v>
       </c>
@@ -8686,7 +8722,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="61.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>474</v>
       </c>
@@ -8700,7 +8736,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>476</v>
       </c>
@@ -8733,1573 +8769,1609 @@
       <c r="H44" s="4" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I44" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="78.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>544</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="P52" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>544</v>
+        <v>555</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>545</v>
+        <v>556</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>552</v>
+        <v>563</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>553</v>
+        <v>564</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>554</v>
+        <v>565</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>558</v>
+        <v>569</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>559</v>
+        <v>570</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>560</v>
+        <v>571</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>561</v>
+        <v>572</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>563</v>
+        <v>574</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>567</v>
+        <v>578</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>569</v>
+        <v>580</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>570</v>
+        <v>581</v>
       </c>
       <c r="O54" s="4" t="s">
-        <v>571</v>
+        <v>582</v>
       </c>
       <c r="P54" s="4" t="s">
-        <v>572</v>
+        <v>583</v>
       </c>
       <c r="Q54" s="4" t="s">
-        <v>573</v>
+        <v>584</v>
       </c>
       <c r="R54" s="4" t="s">
-        <v>574</v>
+        <v>585</v>
       </c>
       <c r="S54" s="4" t="s">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="T54" s="4" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>578</v>
+        <v>589</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>579</v>
+        <v>590</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>580</v>
+        <v>591</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>583</v>
+        <v>594</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>584</v>
+        <v>595</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>585</v>
+        <v>596</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>586</v>
+        <v>597</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>588</v>
+        <v>599</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>594</v>
+        <v>605</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>595</v>
+        <v>606</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>596</v>
+        <v>607</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="150.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>598</v>
+        <v>609</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>599</v>
+        <v>610</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>600</v>
+        <v>611</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>601</v>
+        <v>612</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>602</v>
+        <v>613</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>603</v>
+        <v>614</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>604</v>
+        <v>615</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>605</v>
+        <v>616</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>606</v>
+        <v>617</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>607</v>
+        <v>618</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>608</v>
+        <v>619</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>609</v>
+        <v>620</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>610</v>
+        <v>621</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>611</v>
+        <v>622</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>612</v>
+        <v>623</v>
       </c>
       <c r="P58" s="4" t="s">
-        <v>613</v>
+        <v>624</v>
       </c>
       <c r="Q58" s="4" t="s">
-        <v>614</v>
+        <v>625</v>
       </c>
       <c r="R58" s="4" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="73.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>616</v>
+        <v>627</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>617</v>
+        <v>628</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>618</v>
+        <v>629</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>619</v>
+        <v>630</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="73.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>621</v>
+        <v>632</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>622</v>
+        <v>633</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>623</v>
+        <v>634</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>624</v>
+        <v>635</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>625</v>
+        <v>636</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>627</v>
+        <v>638</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>628</v>
+        <v>639</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>629</v>
+        <v>640</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>630</v>
+        <v>641</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>631</v>
+        <v>642</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>632</v>
+        <v>643</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>633</v>
+        <v>644</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>634</v>
+        <v>645</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>635</v>
+        <v>646</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>636</v>
+        <v>647</v>
       </c>
       <c r="K61" s="4" t="s">
-        <v>637</v>
+        <v>648</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>638</v>
+        <v>649</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>639</v>
+        <v>650</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>640</v>
+        <v>651</v>
       </c>
       <c r="O61" s="4" t="s">
-        <v>641</v>
+        <v>652</v>
       </c>
       <c r="P61" s="4" t="s">
-        <v>642</v>
+        <v>653</v>
       </c>
       <c r="Q61" s="4" t="s">
-        <v>643</v>
+        <v>654</v>
       </c>
       <c r="R61" s="4" t="s">
-        <v>644</v>
+        <v>655</v>
       </c>
       <c r="S61" s="4" t="s">
-        <v>645</v>
+        <v>656</v>
       </c>
       <c r="T61" s="4" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="162" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>647</v>
+        <v>658</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>648</v>
+        <v>659</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>649</v>
+        <v>660</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>650</v>
+        <v>661</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>651</v>
+        <v>662</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>652</v>
+        <v>663</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>653</v>
+        <v>664</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>654</v>
+        <v>665</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>655</v>
+        <v>666</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>656</v>
+        <v>667</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>657</v>
+        <v>668</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>658</v>
+        <v>669</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>659</v>
+        <v>670</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>660</v>
+        <v>671</v>
       </c>
       <c r="O62" s="4" t="s">
-        <v>661</v>
+        <v>672</v>
       </c>
       <c r="P62" s="4" t="s">
-        <v>662</v>
+        <v>673</v>
       </c>
       <c r="Q62" s="4" t="s">
-        <v>663</v>
+        <v>674</v>
       </c>
       <c r="R62" s="4" t="s">
-        <v>664</v>
+        <v>675</v>
       </c>
       <c r="S62" s="4" t="s">
-        <v>665</v>
+        <v>676</v>
       </c>
       <c r="T62" s="4" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>667</v>
+        <v>678</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>668</v>
+        <v>679</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>669</v>
+        <v>680</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>670</v>
+        <v>681</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>671</v>
+        <v>682</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>672</v>
+        <v>683</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>673</v>
+        <v>684</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>674</v>
+        <v>685</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>675</v>
+        <v>686</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>676</v>
+        <v>687</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>677</v>
+        <v>688</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>678</v>
+        <v>689</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>680</v>
+        <v>691</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>681</v>
+        <v>692</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>683</v>
+        <v>694</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>684</v>
+        <v>695</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>685</v>
+        <v>696</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>686</v>
+        <v>697</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>687</v>
+        <v>698</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>688</v>
+        <v>699</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>689</v>
+        <v>700</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>690</v>
+        <v>701</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>691</v>
+        <v>702</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="138.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>693</v>
+        <v>704</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>694</v>
+        <v>705</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>695</v>
+        <v>706</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>696</v>
+        <v>707</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>697</v>
+        <v>708</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>698</v>
+        <v>709</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>700</v>
+        <v>711</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>701</v>
+        <v>712</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>702</v>
+        <v>713</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>703</v>
+        <v>714</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>704</v>
+        <v>715</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="78.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>734</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>737</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>740</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>741</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>742</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>746</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>747</v>
+      </c>
+      <c r="P70" s="4" t="s">
+        <v>748</v>
+      </c>
+      <c r="Q70" s="4" t="s">
+        <v>749</v>
+      </c>
+      <c r="R70" s="4" t="s">
+        <v>750</v>
+      </c>
+      <c r="S70" s="4" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>753</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>701</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>707</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>708</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>709</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>710</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>711</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="K68" s="4" t="s">
-        <v>715</v>
-      </c>
-      <c r="L68" s="4" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
-        <v>717</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>718</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>719</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="162" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3" t="s">
-        <v>721</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>722</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>723</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>725</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>726</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>727</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>728</v>
-      </c>
-      <c r="I70" s="4" t="s">
-        <v>729</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>730</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>731</v>
-      </c>
-      <c r="L70" s="4" t="s">
-        <v>732</v>
-      </c>
-      <c r="M70" s="4" t="s">
-        <v>733</v>
-      </c>
-      <c r="N70" s="4" t="s">
-        <v>734</v>
-      </c>
-      <c r="O70" s="4" t="s">
-        <v>735</v>
-      </c>
-      <c r="P70" s="4" t="s">
-        <v>736</v>
-      </c>
-      <c r="Q70" s="4" t="s">
-        <v>737</v>
-      </c>
-      <c r="R70" s="4" t="s">
-        <v>738</v>
-      </c>
-      <c r="S70" s="4" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
-        <v>740</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>741</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>695</v>
-      </c>
       <c r="D71" s="4" t="s">
-        <v>742</v>
+        <v>754</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>743</v>
+        <v>755</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>744</v>
+        <v>756</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>745</v>
+        <v>757</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>746</v>
+        <v>758</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>747</v>
+        <v>759</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>749</v>
+        <v>761</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>750</v>
+        <v>762</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>751</v>
+        <v>763</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>752</v>
+        <v>764</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="146.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>754</v>
+        <v>766</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>755</v>
+        <v>767</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>756</v>
+        <v>768</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>757</v>
+        <v>769</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>758</v>
+        <v>770</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>759</v>
+        <v>771</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>760</v>
+        <v>772</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>761</v>
+        <v>773</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>762</v>
+        <v>774</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>763</v>
+        <v>775</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>765</v>
+        <v>777</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>766</v>
+        <v>778</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>767</v>
+        <v>779</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>768</v>
+        <v>780</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>769</v>
+        <v>781</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>770</v>
+        <v>782</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>771</v>
+        <v>783</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>772</v>
+        <v>784</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>773</v>
+        <v>785</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>774</v>
+        <v>786</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>775</v>
+        <v>787</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>777</v>
+        <v>789</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>778</v>
+        <v>790</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>779</v>
+        <v>791</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>780</v>
+        <v>792</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>781</v>
+        <v>793</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>782</v>
+        <v>794</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>783</v>
+        <v>795</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>784</v>
+        <v>796</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>785</v>
+        <v>797</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>786</v>
+        <v>798</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>788</v>
+        <v>800</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>789</v>
+        <v>801</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="134.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>791</v>
+        <v>803</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>792</v>
+        <v>804</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>793</v>
+        <v>805</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>794</v>
+        <v>806</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="61.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>796</v>
+        <v>808</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>797</v>
+        <v>809</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>798</v>
+        <v>810</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>799</v>
+        <v>811</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>800</v>
+        <v>812</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>801</v>
+        <v>813</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>802</v>
+        <v>814</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>803</v>
+        <v>815</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>804</v>
+        <v>816</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>805</v>
+        <v>817</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>806</v>
+        <v>818</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>807</v>
+        <v>819</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>809</v>
+        <v>821</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>810</v>
+        <v>822</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>811</v>
+        <v>823</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>812</v>
+        <v>824</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>813</v>
+        <v>825</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>814</v>
+        <v>826</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>816</v>
+        <v>828</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>817</v>
+        <v>829</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>818</v>
+        <v>830</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>819</v>
+        <v>831</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>820</v>
+        <v>832</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>821</v>
+        <v>833</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>822</v>
+        <v>834</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>823</v>
+        <v>835</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>824</v>
+        <v>836</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>825</v>
+        <v>837</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>827</v>
+        <v>839</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>828</v>
+        <v>840</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>829</v>
+        <v>841</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>830</v>
+        <v>842</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>831</v>
+        <v>843</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>832</v>
+        <v>844</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>833</v>
+        <v>845</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>834</v>
+        <v>846</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>835</v>
+        <v>847</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>836</v>
+        <v>848</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>837</v>
+        <v>849</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>838</v>
+        <v>850</v>
       </c>
       <c r="M81" s="4" t="s">
-        <v>839</v>
+        <v>851</v>
       </c>
       <c r="N81" s="4" t="s">
-        <v>840</v>
+        <v>852</v>
       </c>
       <c r="O81" s="4" t="s">
-        <v>841</v>
+        <v>853</v>
       </c>
       <c r="P81" s="4" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>843</v>
+        <v>855</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>844</v>
+        <v>856</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>845</v>
+        <v>857</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>846</v>
+        <v>858</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>847</v>
+        <v>859</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>848</v>
+        <v>860</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>849</v>
+        <v>861</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="110" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>851</v>
+        <v>863</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>852</v>
+        <v>864</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>853</v>
+        <v>865</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>854</v>
+        <v>866</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>855</v>
+        <v>867</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>857</v>
+        <v>869</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>858</v>
+        <v>870</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>859</v>
+        <v>871</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>860</v>
+        <v>872</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>861</v>
+        <v>873</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>862</v>
+        <v>874</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>863</v>
+        <v>875</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>865</v>
+        <v>877</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>866</v>
+        <v>878</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>867</v>
+        <v>879</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>868</v>
+        <v>880</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>869</v>
+        <v>881</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>870</v>
+        <v>882</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>871</v>
+        <v>883</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>872</v>
+        <v>884</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>873</v>
+        <v>885</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>874</v>
+        <v>886</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>875</v>
+        <v>887</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>876</v>
+        <v>888</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>877</v>
+        <v>889</v>
       </c>
       <c r="N85" s="4" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="150.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>879</v>
+        <v>891</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>880</v>
+        <v>892</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="122.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>882</v>
+        <v>894</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>883</v>
+        <v>895</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>884</v>
+        <v>896</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>885</v>
+        <v>897</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>886</v>
+        <v>898</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>887</v>
+        <v>899</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>888</v>
+        <v>900</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>890</v>
+        <v>902</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>891</v>
+        <v>903</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>892</v>
+        <v>904</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>893</v>
+        <v>905</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>894</v>
+        <v>906</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>895</v>
+        <v>907</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>896</v>
+        <v>908</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="170.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>897</v>
+        <v>909</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>898</v>
+        <v>910</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>899</v>
+        <v>911</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>900</v>
+        <v>912</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>901</v>
+        <v>913</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>902</v>
+        <v>914</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>903</v>
+        <v>915</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>904</v>
+        <v>916</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>905</v>
+        <v>917</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>906</v>
+        <v>918</v>
       </c>
       <c r="K89" s="4" t="s">
-        <v>907</v>
+        <v>919</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>908</v>
+        <v>920</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>909</v>
+        <v>921</v>
       </c>
       <c r="N89" s="4" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
       <c r="O89" s="4" t="s">
-        <v>911</v>
+        <v>923</v>
       </c>
       <c r="P89" s="4" t="s">
-        <v>912</v>
+        <v>924</v>
       </c>
       <c r="Q89" s="4" t="s">
-        <v>913</v>
+        <v>925</v>
       </c>
       <c r="R89" s="4" t="s">
-        <v>914</v>
+        <v>926</v>
       </c>
       <c r="S89" s="4" t="s">
-        <v>915</v>
+        <v>927</v>
       </c>
       <c r="T89" s="4" t="s">
-        <v>916</v>
+        <v>928</v>
       </c>
       <c r="U89" s="4" t="s">
-        <v>917</v>
+        <v>929</v>
       </c>
       <c r="V89" s="4" t="s">
-        <v>918</v>
+        <v>930</v>
       </c>
       <c r="W89" s="4" t="s">
-        <v>919</v>
+        <v>931</v>
       </c>
       <c r="X89" s="4" t="s">
-        <v>920</v>
+        <v>932</v>
       </c>
       <c r="Y89" s="4" t="s">
-        <v>921</v>
+        <v>933</v>
       </c>
       <c r="Z89" s="4" t="s">
-        <v>922</v>
+        <v>934</v>
       </c>
       <c r="AA89" s="4" t="s">
-        <v>923</v>
+        <v>935</v>
       </c>
       <c r="AB89" s="4" t="s">
-        <v>924</v>
+        <v>936</v>
       </c>
       <c r="AC89" s="4" t="s">
-        <v>925</v>
+        <v>937</v>
       </c>
       <c r="AD89" s="4" t="s">
-        <v>926</v>
+        <v>938</v>
       </c>
       <c r="AE89" s="4" t="s">
-        <v>927</v>
+        <v>939</v>
       </c>
       <c r="AF89" s="4" t="s">
-        <v>928</v>
+        <v>940</v>
       </c>
       <c r="AG89" s="4" t="s">
-        <v>929</v>
+        <v>941</v>
       </c>
       <c r="AH89" s="4" t="s">
-        <v>930</v>
+        <v>942</v>
       </c>
       <c r="AI89" s="4" t="s">
-        <v>931</v>
+        <v>943</v>
       </c>
       <c r="AJ89" s="4" t="s">
-        <v>932</v>
+        <v>944</v>
       </c>
       <c r="AK89" s="4" t="s">
-        <v>933</v>
+        <v>945</v>
       </c>
       <c r="AL89" s="4" t="s">
-        <v>934</v>
+        <v>946</v>
       </c>
       <c r="AM89" s="4" t="s">
-        <v>935</v>
+        <v>947</v>
       </c>
       <c r="AN89" s="4" t="s">
-        <v>936</v>
+        <v>948</v>
       </c>
       <c r="AO89" s="4" t="s">
-        <v>937</v>
+        <v>949</v>
       </c>
       <c r="AP89" s="4" t="s">
-        <v>938</v>
+        <v>950</v>
       </c>
       <c r="AQ89" s="4" t="s">
-        <v>939</v>
+        <v>951</v>
       </c>
       <c r="AR89" s="4" t="s">
-        <v>940</v>
+        <v>952</v>
       </c>
       <c r="AS89" s="4" t="s">
-        <v>941</v>
+        <v>953</v>
       </c>
       <c r="AT89" s="2" t="s">
-        <v>942</v>
+        <v>954</v>
       </c>
       <c r="AU89" s="4" t="s">
-        <v>943</v>
+        <v>955</v>
       </c>
       <c r="AV89" s="4" t="s">
-        <v>944</v>
+        <v>956</v>
       </c>
       <c r="AW89" s="4" t="s">
-        <v>945</v>
+        <v>957</v>
       </c>
       <c r="AX89" s="4" t="s">
-        <v>946</v>
+        <v>958</v>
       </c>
       <c r="AY89" s="4" t="s">
-        <v>947</v>
+        <v>959</v>
       </c>
       <c r="AZ89" s="4" t="s">
-        <v>948</v>
+        <v>960</v>
       </c>
       <c r="BA89" s="2" t="s">
-        <v>949</v>
+        <v>961</v>
       </c>
       <c r="BB89" s="4" t="s">
-        <v>950</v>
+        <v>962</v>
       </c>
       <c r="BC89" s="4" t="s">
-        <v>951</v>
+        <v>963</v>
       </c>
       <c r="BD89" s="4" t="s">
-        <v>952</v>
+        <v>964</v>
       </c>
       <c r="BE89" s="4" t="s">
-        <v>953</v>
+        <v>965</v>
       </c>
       <c r="BF89" s="4" t="s">
-        <v>954</v>
+        <v>966</v>
       </c>
       <c r="BG89" s="4" t="s">
-        <v>955</v>
+        <v>967</v>
       </c>
       <c r="BH89" s="4" t="s">
-        <v>956</v>
+        <v>968</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="97.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>957</v>
+        <v>969</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>958</v>
+        <v>970</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="85.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>959</v>
+        <v>971</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>960</v>
+        <v>972</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>961</v>
+        <v>973</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>962</v>
+        <v>974</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>963</v>
+        <v>975</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>964</v>
+        <v>976</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>965</v>
+        <v>977</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>966</v>
+        <v>978</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="61.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>967</v>
+        <v>979</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>968</v>
+        <v>980</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="61.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>969</v>
+        <v>981</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>970</v>
+        <v>982</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>971</v>
+        <v>983</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>972</v>
+        <v>984</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>973</v>
+        <v>985</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10433,18 +10505,19 @@
   </sheetPr>
   <dimension ref="A1:U114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="2" style="0" width="23.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>974</v>
+        <v>986</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -10509,569 +10582,569 @@
     </row>
     <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>975</v>
+        <v>987</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>976</v>
+        <v>988</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>977</v>
+        <v>989</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>978</v>
+        <v>990</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>979</v>
+        <v>991</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>980</v>
+        <v>992</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>981</v>
+        <v>993</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>982</v>
+        <v>994</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>983</v>
+        <v>995</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>984</v>
+        <v>996</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>985</v>
+        <v>997</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>986</v>
+        <v>998</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>987</v>
+        <v>999</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>988</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>989</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>990</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>991</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>992</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>993</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>994</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>995</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>996</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>997</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>998</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>999</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>1000</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>1001</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>1002</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>1003</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>1004</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>1005</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>1006</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>1007</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>1008</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>1009</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>1010</v>
+        <v>1022</v>
       </c>
       <c r="B37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>1011</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>1012</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>1013</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>1014</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>1015</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>1016</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>1017</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>1018</v>
+        <v>1030</v>
       </c>
       <c r="B45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>1019</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>1020</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>1021</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>1022</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>1023</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>1024</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>1025</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>1026</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>1027</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>1028</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>1029</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>1030</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>1031</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>1032</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>1033</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>1034</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>1035</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>1036</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>1037</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>1038</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>1039</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>1040</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>1041</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>1042</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>1043</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>1044</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>1045</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>1046</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>1047</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>1048</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>1049</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>1050</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>1051</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>1052</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>1053</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>1054</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>1055</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
-        <v>1056</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>1057</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>1058</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>1059</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>1060</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>1061</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="s">
-        <v>1062</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="s">
-        <v>1063</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="s">
-        <v>1064</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="6" t="s">
-        <v>1065</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
-        <v>1066</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="s">
-        <v>1067</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="s">
-        <v>1068</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
-        <v>1069</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="s">
-        <v>1070</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="s">
-        <v>1071</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="6" t="s">
-        <v>1072</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
-        <v>1073</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="6" t="s">
-        <v>1074</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="6" t="s">
-        <v>1075</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="s">
-        <v>1076</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="6" t="s">
-        <v>1077</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="6" t="s">
-        <v>1078</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="s">
-        <v>1079</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="6" t="s">
-        <v>1080</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="6" t="s">
-        <v>1081</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="6" t="s">
-        <v>1082</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
-        <v>1083</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="6" t="s">
-        <v>1084</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="6" t="s">
-        <v>1085</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="6" t="s">
-        <v>1086</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="6" t="s">
-        <v>1087</v>
+        <v>1099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>